<commit_message>
text & data-time functions
</commit_message>
<xml_diff>
--- a/Excel-Homework-Exercises-ANSWERS.xlsx
+++ b/Excel-Homework-Exercises-ANSWERS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/GodSpeed/Documents/CodeWork/excelAdvancedFormulas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B311BF-B2EF-8040-803A-95586CD76B8A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C99F3A28-D828-8645-943F-49E9F6E5DC5C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="709" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="709" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Formulas 101" sheetId="19" r:id="rId1"/>
@@ -7559,7 +7559,7 @@
       </c>
       <c r="C3" s="53">
         <f ca="1">TODAY()</f>
-        <v>43379</v>
+        <v>43380</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -7568,7 +7568,7 @@
       </c>
       <c r="C4" s="54">
         <f ca="1">NOW()</f>
-        <v>43379.893438310188</v>
+        <v>43380.881669560185</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -7602,7 +7602,7 @@
       </c>
       <c r="D7" s="55">
         <f ca="1">DAY(C3)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E7" s="55">
         <f ca="1">HOUR(C4)</f>
@@ -7610,11 +7610,11 @@
       </c>
       <c r="F7" s="55">
         <f ca="1">MINUTE(C4)</f>
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="G7" s="55">
         <f ca="1">SECOND(C4)</f>
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -7632,7 +7632,7 @@
       </c>
       <c r="C9" s="56">
         <f ca="1">WEEKDAY(C3)</f>
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -10060,7 +10060,7 @@
   </sheetPr>
   <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -20364,7 +20364,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20599,7 +20599,7 @@
   </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>

</xml_diff>